<commit_message>
Modified prox design, added BOM
</commit_message>
<xml_diff>
--- a/Documentation/tools_BOM.xlsx
+++ b/Documentation/tools_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>Column10</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Programmer</t>
-  </si>
-  <si>
     <t>Protoboard</t>
   </si>
   <si>
@@ -96,18 +93,6 @@
     <t>https://www.sparkfun.com/products/115</t>
   </si>
   <si>
-    <t>PRT-08619</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8619?</t>
-  </si>
-  <si>
-    <t>BOB-00718</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/718</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -145,6 +130,84 @@
   </si>
   <si>
     <t>https://www.sparkfun.com/products/8230</t>
+  </si>
+  <si>
+    <t>Programmer/Uno</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>DEV-11021</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11021</t>
+  </si>
+  <si>
+    <t>Bus Pirate</t>
+  </si>
+  <si>
+    <t>TOL-09544</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9544</t>
+  </si>
+  <si>
+    <t>DEV-07914</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/7914?</t>
+  </si>
+  <si>
+    <t>Bus Pirate Cable</t>
+  </si>
+  <si>
+    <t>CAB-09556</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9556</t>
+  </si>
+  <si>
+    <t>Hook-up Wire</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>PRT-08022</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8022</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>PRT-08026</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8026</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>PRT-08025</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8025</t>
+  </si>
+  <si>
+    <t>25'</t>
+  </si>
+  <si>
+    <t>Solder</t>
+  </si>
+  <si>
+    <t>TOL-09161</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9161</t>
   </si>
 </sst>
 </file>
@@ -263,6 +326,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K19" totalsRowShown="0">
   <autoFilter ref="A1:K19"/>
+  <sortState ref="A2:K19">
+    <sortCondition ref="A2:A19"/>
+    <sortCondition ref="F2:F19"/>
+    <sortCondition ref="K2:K19"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="Part"/>
     <tableColumn id="15" name="Description"/>
@@ -573,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,144 +712,144 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1">
-        <v>14.95</v>
+        <v>21</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1.5</v>
       </c>
       <c r="J2" s="3">
         <v>1</v>
       </c>
       <c r="K2" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>14.95</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1">
-        <v>9.9499999999999993</v>
+        <v>44</v>
+      </c>
+      <c r="I3" s="5">
+        <v>29.95</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
       </c>
       <c r="K3" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>9.9499999999999993</v>
+        <v>29.95</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="3">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1.5</v>
+        <v>49</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4.95</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>1.5</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3">
-        <v>40</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1.5</v>
+        <v>31</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1.95</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>1.5</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I6" s="5">
         <v>0.45</v>
@@ -796,182 +864,247 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="I7" s="5">
-        <v>0.45</v>
+        <v>2.5</v>
       </c>
       <c r="J7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="3">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="I8" s="5">
-        <v>1.95</v>
+        <v>2.5</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
       <c r="K8" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>1.95</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="I9" s="5">
-        <v>0</v>
+        <v>2.95</v>
       </c>
       <c r="J9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1">
-        <v>0</v>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.45</v>
       </c>
       <c r="J10" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3">
+        <v>40</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5">
-        <v>0</v>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.5</v>
       </c>
       <c r="J11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5">
-        <v>0</v>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1">
+        <v>29.95</v>
       </c>
       <c r="J12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>29.95</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5">
-        <v>0</v>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="1">
+        <v>9.9499999999999993</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="I14" s="5">
-        <v>0</v>
+        <v>5.95</v>
       </c>
       <c r="J14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1059,7 +1192,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7">
         <f>SUM(Table3[Total])</f>
-        <v>31.199999999999996</v>
+        <v>95.000000000000014</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1225,21 +1358,26 @@
     <row r="182" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
-    <hyperlink ref="H8" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="G7" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="H6" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="H10" r:id="rId5"/>
+    <hyperlink ref="G10" r:id="rId6"/>
+    <hyperlink ref="G6" r:id="rId7"/>
+    <hyperlink ref="H6" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G3" r:id="rId10"/>
+    <hyperlink ref="G13" r:id="rId11"/>
+    <hyperlink ref="G4" r:id="rId12"/>
+    <hyperlink ref="G7" r:id="rId13"/>
+    <hyperlink ref="G9" r:id="rId14"/>
+    <hyperlink ref="G14" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>